<commit_message>
Excel optional columns and minor fixes (#3)
Squashed commit of the following:

commit 7b52f7125930f68720eb40c8105543643b10754e
Author: Panagiotis Bochalis <bochalito@gmail.com>
Date:   Mon Apr 23 16:35:48 2018 +0300

    Number type input in access code info

commit 5b58194c10229771cc038bd37ba77a0206a404aa
Author: John Buluba <buluba89@gmail.com>
Date:   Mon Apr 23 16:29:18 2018 +0300

    db specific migrations

commit 2d69bf5f9696bf8e464a018a02a04b039509cd21
Author: Panagiotis Bochalis <bochalito@gmail.com>
Date:   Fri Apr 20 16:55:14 2018 +0300

    redirect error on navbar fixed

commit 9f7e869e64af90667b9b26e0161aa5621480c80c
Author: John Buluba <buluba89@gmail.com>
Date:   Mon Apr 23 15:08:59 2018 +0300

    Fixed null value in isActivated

commit 33f4d847449d1f8f446cbc06d07e229f43223b68
Author: John Buluba <buluba89@gmail.com>
Date:   Fri Apr 20 17:33:20 2018 +0300

    Fixed depedency issue and excel parser fixes
</commit_message>
<xml_diff>
--- a/licenser-integration-tests/src/test/resources/fixtures/valid.xlsx
+++ b/licenser-integration-tests/src/test/resources/fixtures/valid.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>access_code</t>
   </si>
@@ -29,16 +29,10 @@
     <t>duration</t>
   </si>
   <si>
-    <t>is_activated</t>
-  </si>
-  <si>
     <t>test1</t>
   </si>
   <si>
     <t>test2</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -135,7 +129,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -159,13 +153,10 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -179,7 +170,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -189,9 +180,6 @@
       </c>
       <c r="D3" s="0" t="n">
         <v>30</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>